<commit_message>
Second testcase run successfully
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\old\D\SeleniumUdemy\SeleniumTesting\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaga\git\repository\DataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{155A2A28-CB79-4DDA-81E7-97A23819037E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AE38F8-6E0E-4B62-AEAA-25E59F0088F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5943E7F4-AE9E-4516-8C4B-69826B6FDD0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,6 +31,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>thamil</t>
+  </si>
+  <si>
+    <t>alagan</t>
+  </si>
+  <si>
+    <t>b27 a93</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,14 +409,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AFF1E8F-4479-449C-AF79-BCA92BEB8039}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="25.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>